<commit_message>
ready to do SE
</commit_message>
<xml_diff>
--- a/circuits/ind_feeder.xlsx
+++ b/circuits/ind_feeder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harshil\Desktop\4thyear\python\final code\circuits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932F1B0C-F789-476A-973F-5C17C157F622}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED4E40E-C6D4-4E85-8805-D178708ED9FD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1170" windowWidth="28800" windowHeight="8130" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dtypes" sheetId="1" r:id="rId1"/>
@@ -53,6 +53,7 @@
     <sheet name="res_dcline" sheetId="38" r:id="rId38"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -10411,7 +10412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
@@ -10773,7 +10774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:U66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>